<commit_message>
changed StableMotifs -->  PyStableMotifs and reran the notebooks for testing. I'm commiting the outputs as well.
</commit_message>
<xml_diff>
--- a/timing_results.xlsx
+++ b/timing_results.xlsx
@@ -369,42 +369,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Pint</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>CABEAN</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PyBoolNet_Asp</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>stable_motifs_new</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>bioLQM</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>PyBoolNet_Asp</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>boolsim</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>sm_jgtz</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>PyBoolNet</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>boolsim</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>sm_jgtz</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Pint</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>CABEAN</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>stable_motifs_new</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
@@ -418,28 +418,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.3042127349999646</v>
+        <v>0.1798734390013124</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1132306829995287</v>
+        <v>0.07706998499998008</v>
       </c>
       <c r="D2" t="n">
-        <v>0.3926209190003647</v>
+        <v>0.09504505499899096</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1661090769994189</v>
+        <v>0.6167890689994238</v>
       </c>
       <c r="F2" t="n">
-        <v>31.46968757600007</v>
+        <v>0.127908569000283</v>
       </c>
       <c r="G2" t="n">
-        <v>0.09880145700026333</v>
+        <v>0.1977810940006748</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1332884160001413</v>
+        <v>31.96101380100117</v>
       </c>
       <c r="I2" t="n">
-        <v>0.6029262719994222</v>
+        <v>0.3814105519995792</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
nothing new, just the results of the last test run present in the notebook
</commit_message>
<xml_diff>
--- a/timing_results.xlsx
+++ b/timing_results.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -369,45 +369,40 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>pyboolnet</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Pint</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>boolsim</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>stablemotifs2013</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>bioLQM</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>CABEAN</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>PyBoolNet_Asp</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>stable_motifs_new</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>bioLQM</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>boolsim</t>
-        </is>
-      </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>sm_jgtz</t>
+          <t>pystablemotifs</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>PyBoolNet</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>model</t>
         </is>
@@ -418,30 +413,27 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1798734390013124</v>
+        <v>0.5727500239991059</v>
       </c>
       <c r="C2" t="n">
-        <v>0.07706998499998008</v>
+        <v>0.3547523589986668</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09504505499899096</v>
+        <v>0.2571681939989503</v>
       </c>
       <c r="E2" t="n">
-        <v>0.6167890689994238</v>
+        <v>59.29691573200034</v>
       </c>
       <c r="F2" t="n">
-        <v>0.127908569000283</v>
+        <v>0.1880386279990489</v>
       </c>
       <c r="G2" t="n">
-        <v>0.1977810940006748</v>
+        <v>0.1789524010018795</v>
       </c>
       <c r="H2" t="n">
-        <v>31.96101380100117</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.3814105519995792</v>
-      </c>
-      <c r="J2" t="inlineStr">
+        <v>0.9352700599993113</v>
+      </c>
+      <c r="I2" t="inlineStr">
         <is>
           <t>phase_switch</t>
         </is>

</xml_diff>